<commit_message>
fms commit facility management
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_FMS_Ajith/TestData/FMSTestData.xlsx
+++ b/AzentioAutomationFramework_FMS_Ajith/TestData/FMSTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" tabRatio="971" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" tabRatio="971" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="AllFeaturesTestExecutionInfo" sheetId="8" r:id="rId1"/>
@@ -14,15 +14,16 @@
     <sheet name="FMSParam_login" sheetId="2" r:id="rId5"/>
     <sheet name="FMS_Login" sheetId="1" r:id="rId6"/>
     <sheet name="SadsLogin" sheetId="3" r:id="rId7"/>
-    <sheet name="ApplicationForFinancialFacility" sheetId="11" r:id="rId8"/>
-    <sheet name="TestExecution" sheetId="7" r:id="rId9"/>
+    <sheet name="FacilitiesManagement" sheetId="12" r:id="rId8"/>
+    <sheet name="ApplicationForFinancialFacility" sheetId="11" r:id="rId9"/>
+    <sheet name="TestExecution" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="124">
   <si>
     <t>Password</t>
   </si>
@@ -286,10 +287,118 @@
     <t>999999999999999</t>
   </si>
   <si>
-    <t>AFFF_01</t>
-  </si>
-  <si>
-    <t>AFFF_01_D1</t>
+    <t>AT_FM_010</t>
+  </si>
+  <si>
+    <t>AT_FM_010_D1</t>
+  </si>
+  <si>
+    <t>SearchStatus</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>AT_AFF_004</t>
+  </si>
+  <si>
+    <t>SectorCode</t>
+  </si>
+  <si>
+    <t>BriefName</t>
+  </si>
+  <si>
+    <t>AT_AFF_004_01</t>
+  </si>
+  <si>
+    <t>AT_AFF_004_02</t>
+  </si>
+  <si>
+    <t>AT_AFF_004_01_D1</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>AT_AFF_024</t>
+  </si>
+  <si>
+    <t>AT_AFF_024_D1</t>
+  </si>
+  <si>
+    <t>AT_AFF_008</t>
+  </si>
+  <si>
+    <t>AT_AFF_008_D1</t>
+  </si>
+  <si>
+    <t>ReasonForSubmission</t>
+  </si>
+  <si>
+    <t>New Request</t>
+  </si>
+  <si>
+    <t>CIFNO</t>
+  </si>
+  <si>
+    <t>FacilityType</t>
+  </si>
+  <si>
+    <t>TotalLimit</t>
+  </si>
+  <si>
+    <t>ProductClass</t>
+  </si>
+  <si>
+    <t>MarginValue</t>
+  </si>
+  <si>
+    <t>RequestID</t>
+  </si>
+  <si>
+    <t>DecisionField</t>
+  </si>
+  <si>
+    <t>Forward</t>
+  </si>
+  <si>
+    <t>Approval Committee</t>
+  </si>
+  <si>
+    <t>Recommendation</t>
+  </si>
+  <si>
+    <t>AT_AFF_019</t>
+  </si>
+  <si>
+    <t>AT_AFF_019_D1</t>
+  </si>
+  <si>
+    <t>CollateralType</t>
+  </si>
+  <si>
+    <t>BriefDescription</t>
+  </si>
+  <si>
+    <t>LongDescription</t>
+  </si>
+  <si>
+    <t>Test Collateral</t>
+  </si>
+  <si>
+    <t>CollateralCurrency</t>
+  </si>
+  <si>
+    <t>Investment Committee</t>
+  </si>
+  <si>
+    <t>4364</t>
+  </si>
+  <si>
+    <t>896</t>
+  </si>
+  <si>
+    <t>762</t>
   </si>
 </sst>
 </file>
@@ -300,7 +409,7 @@
     <numFmt numFmtId="164" formatCode="&quot;Rs.&quot;#,##0.00;[Red]\-&quot;Rs.&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -377,8 +486,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -439,8 +554,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -478,6 +599,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -493,7 +638,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -518,7 +663,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -568,6 +712,16 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="10" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Excel Built-in Normal" xfId="7"/>
@@ -906,7 +1060,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -922,197 +1076,430 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="18.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.7109375" style="32" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="28.85546875" style="3" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="19.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="11.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="27.7109375" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" style="3" width="18.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="31" width="17.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="3" width="15.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="3" width="18.140625" collapsed="true"/>
+    <col min="9" max="16384" style="3" width="28.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="18" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23">
-        <v>1</v>
-      </c>
-      <c r="H2" s="24"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="22">
+        <v>1</v>
+      </c>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="31"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="4.5870078740157476" bottom="4.5870078740157476" header="4.3901574803149597" footer="4.3901574803149597"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="40" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="9.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="13.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="15.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="14.5703125" collapsed="true"/>
+    <col min="5" max="6" bestFit="true" customWidth="true" style="4" width="26.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="4" width="28.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="4" width="27.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="4" width="26.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="4" width="25.85546875" collapsed="true"/>
+    <col min="11" max="16384" style="4" width="40.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A3" s="6"/>
+      <c r="B3" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="6"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="6"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="6"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="6"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="6"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D7:D11 D2:D5 C5 C2">
+    <cfRule type="containsText" dxfId="1" priority="9" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="10" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",C2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D11">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="8.7188976377952763" bottom="8.7188976377952763" header="8.5220472440944892" footer="8.5220472440944892"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -1126,56 +1513,56 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="123" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="123" style="3" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="18.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="30.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="38.42578125" collapsed="true"/>
+    <col min="4" max="16384" style="3" width="123.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="32" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30">
-      <c r="A2" s="34"/>
-      <c r="B2" s="24" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="37" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30">
-      <c r="A3" s="35"/>
-      <c r="B3" s="24" t="s">
+      <c r="A3" s="34"/>
+      <c r="B3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="37" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30">
       <c r="A4" s="6"/>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="37" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30">
       <c r="A5" s="9"/>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="37" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1195,28 +1582,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="34.42578125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.28515625" style="2"/>
+    <col min="1" max="1" customWidth="true" style="2" width="18.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="22.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="21.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="27.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="34.42578125" collapsed="true"/>
+    <col min="6" max="16384" style="2" width="9.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="37" t="s">
+      <c r="D1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="36" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1440,28 +1827,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.28515625" style="2"/>
+    <col min="1" max="1" customWidth="true" style="2" width="22.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="27.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="21.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="18.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="21.42578125" collapsed="true"/>
+    <col min="6" max="16384" style="2" width="9.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="37" t="s">
+      <c r="D1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="36" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1685,28 +2072,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.28515625" style="2"/>
+    <col min="1" max="1" customWidth="true" style="2" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="9.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="11.5703125" collapsed="true"/>
+    <col min="6" max="16384" style="2" width="9.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="36" t="s">
+      <c r="D1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="35" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1930,28 +2317,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.28515625" style="2"/>
+    <col min="1" max="1" customWidth="true" style="2" width="13.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="9.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="14.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="11.5703125" collapsed="true"/>
+    <col min="6" max="16384" style="2" width="9.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="37" t="s">
+      <c r="D1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="36" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2175,20 +2562,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.28515625" style="2"/>
+    <col min="1" max="1" customWidth="true" style="2" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="9.42578125" collapsed="true"/>
+    <col min="4" max="16384" style="2" width="9.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="36" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2224,248 +2611,338 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="39" t="s">
-        <v>84</v>
-      </c>
+      <c r="C1" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:8" ht="15">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="42">
-        <v>727</v>
-      </c>
-      <c r="E2" s="42">
-        <v>369</v>
-      </c>
-      <c r="F2" s="42">
-        <v>320</v>
-      </c>
-      <c r="G2" s="42">
-        <v>2</v>
-      </c>
-      <c r="H2" s="43" t="s">
-        <v>85</v>
-      </c>
+      <c r="C2" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="40" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="13.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="26.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="26.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="25.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="40" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.48828125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="10.484375" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="17.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="12" t="s">
+    <row r="1" spans="1:24" ht="15">
+      <c r="A1" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="M1" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="O1" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="P1" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q1" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="R1" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="S1" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="T1" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="U1" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="V1" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="W1" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="X1" s="44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="15">
+      <c r="A2" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="40"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="K2" s="40"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="48"/>
+      <c r="V2" s="48"/>
+      <c r="W2" s="48"/>
+      <c r="X2" s="48"/>
+    </row>
+    <row r="3" spans="1:24" ht="15">
+      <c r="A3" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="40"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="L3" s="51">
+        <v>727</v>
+      </c>
+      <c r="M3" s="51">
+        <v>221</v>
+      </c>
+      <c r="N3" s="51">
+        <v>10000</v>
+      </c>
+      <c r="O3" s="51">
+        <v>1</v>
+      </c>
+      <c r="P3" s="51">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="R3" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="S3" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="T3" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="U3" s="51"/>
+      <c r="V3" s="51"/>
+      <c r="W3" s="51"/>
+      <c r="X3" s="51"/>
+    </row>
+    <row r="4" spans="1:24" ht="15">
+      <c r="A4" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="40"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="47"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+      <c r="U4" s="51">
         <v>26</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="6">
+      <c r="V4" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="W4" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="X4" s="51">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="15">
+      <c r="A5" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="41">
+        <v>727</v>
+      </c>
+      <c r="E5" s="41">
+        <v>369</v>
+      </c>
+      <c r="F5" s="41">
+        <v>320</v>
+      </c>
+      <c r="G5" s="41">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="6"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="6"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="6"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="6"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
+      <c r="H5" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="I5" s="46"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="49"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="49"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="48"/>
+      <c r="W5" s="48"/>
+      <c r="X5" s="48"/>
+    </row>
+    <row r="6" spans="1:24" ht="15">
+      <c r="A6" s="50"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2 D4:D8">
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",D2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D8">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="8.7188976377952763" bottom="8.7188976377952763" header="8.5220472440944892" footer="8.5220472440944892"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>